<commit_message>
Changes at the 11th hour
</commit_message>
<xml_diff>
--- a/Documentation/ExcelDiagram/Diagram.xlsx
+++ b/Documentation/ExcelDiagram/Diagram.xlsx
@@ -935,11 +935,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="109983744"/>
-        <c:axId val="70412544"/>
+        <c:axId val="84592128"/>
+        <c:axId val="80608576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109983744"/>
+        <c:axId val="84592128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -949,7 +949,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70412544"/>
+        <c:crossAx val="80608576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -957,7 +957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70412544"/>
+        <c:axId val="80608576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,7 +968,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109983744"/>
+        <c:crossAx val="84592128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1731,11 +1731,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="110444544"/>
-        <c:axId val="70414848"/>
+        <c:axId val="58278400"/>
+        <c:axId val="58123968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110444544"/>
+        <c:axId val="58278400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1745,7 +1745,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70414848"/>
+        <c:crossAx val="58123968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1753,7 +1753,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70414848"/>
+        <c:axId val="58123968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -1766,14 +1766,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110444544"/>
+        <c:crossAx val="58278400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2530,11 +2529,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="123204608"/>
-        <c:axId val="123326976"/>
+        <c:axId val="84593152"/>
+        <c:axId val="58126272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="123204608"/>
+        <c:axId val="84593152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2544,7 +2543,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123326976"/>
+        <c:crossAx val="58126272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2552,7 +2551,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="123326976"/>
+        <c:axId val="58126272"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -2590,7 +2589,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123204608"/>
+        <c:crossAx val="84593152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2675,28 +2674,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>1736</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1736</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2707,20 +2706,20 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
+                <c:pt idx="3">
+                  <c:v>5211.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1340.6799999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>335.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>79.91</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>20.03</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>79.91</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>335.29999999999995</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1340.6799999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5211.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2751,28 +2750,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>1736</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1736</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2783,20 +2782,20 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
+                <c:pt idx="3">
+                  <c:v>1999.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>505.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>127.63999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32.380000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>8.4700000000000006</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32.380000000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>127.63999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>505.6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1999.92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2827,28 +2826,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>1736</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1736</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2859,23 +2858,23 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
+                <c:pt idx="2">
+                  <c:v>6279.2800000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1576.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>393.54</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.38999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.61</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>6.25</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24.61</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100.38999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>393.54</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1576.45</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6279.2800000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2906,28 +2905,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>1736</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1736</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2938,26 +2937,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
+                <c:pt idx="1">
+                  <c:v>24254.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6064.38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1529.22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>376.95</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97.62</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>6.08</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>23.999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>97.62</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>376.95</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1529.22</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6064.38</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24254.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2988,28 +2987,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>1736</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1736</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3020,26 +3019,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
+                <c:pt idx="1">
+                  <c:v>23632.469999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5905.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1488.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>368.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95.34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>5.95</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>23.45</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>95.34</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>368.08</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1488.93</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5905.33</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>23632.469999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3070,28 +3069,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>1736</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1736</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3102,26 +3101,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
+                <c:pt idx="1">
+                  <c:v>23889.550000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5962.91</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1483.34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>365.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93.33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.419999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>5.98</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>23.419999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>93.33</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>365.96</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1483.34</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5962.91</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>23889.550000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3152,28 +3151,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>1736</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1736</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3184,26 +3183,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
+                <c:pt idx="1">
+                  <c:v>13465.76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3379.89</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>827.59</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>213.77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54.24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.790000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>3.67</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13.790000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>54.24</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>213.77</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>827.59</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3379.89</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13465.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3234,28 +3233,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>1736</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1736</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3266,26 +3265,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
+                <c:pt idx="1">
+                  <c:v>13096.300000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3281.44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>828.47</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>213.26999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55.22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.780000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>3.5799999999999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13.780000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>55.22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>213.26999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>828.47</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3281.44</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13096.300000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3316,28 +3315,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>1736</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1736</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3348,26 +3347,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
+                <c:pt idx="1">
+                  <c:v>14348.41</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3582.49</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>900.14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>231.64000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58.22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.790000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>3.92</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>14.790000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>58.22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>231.64000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>900.14</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3582.49</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14348.41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3398,28 +3397,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>1736</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1736</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3431,28 +3430,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>34714.71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12003.22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3011.57</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>747.30000000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188.64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48.11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>3.2600000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>48.11</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>188.64</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>747.30000000000007</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3011.57</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12003.22</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34714.71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3469,11 +3468,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="110446592"/>
-        <c:axId val="70417152"/>
+        <c:axId val="58280448"/>
+        <c:axId val="58128576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110446592"/>
+        <c:axId val="58280448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3483,7 +3482,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70417152"/>
+        <c:crossAx val="58128576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3491,7 +3490,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70417152"/>
+        <c:axId val="58128576"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -3503,7 +3502,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110446592"/>
+        <c:crossAx val="58280448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3564,7 +3563,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>1736</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3613,35 +3612,8 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>20.03</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.4700000000000006</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.08</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.95</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.98</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.67</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.5799999999999996</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.92</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.2600000000000002</c:v>
+                  <c:v>34714.71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3657,7 +3629,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3706,35 +3678,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>79.91</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32.380000000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>24.61</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>23.999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>23.45</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>23.419999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13.790000000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>13.780000000000001</c:v>
+                <c:pt idx="3">
+                  <c:v>24254.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23632.469999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23889.550000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13465.76</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13096.300000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14.790000000000001</c:v>
+                  <c:v>14348.41</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.25</c:v>
+                  <c:v>12003.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3750,7 +3713,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>64</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3799,35 +3762,29 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>335.29999999999995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>127.63999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100.38999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>97.62</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>95.34</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>93.33</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>54.24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>55.22</c:v>
+                <c:pt idx="2">
+                  <c:v>6279.2800000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6064.38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5905.33</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5962.91</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3379.89</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3281.44</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>58.22</c:v>
+                  <c:v>3582.49</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>48.11</c:v>
+                  <c:v>3011.57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3843,7 +3800,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>128</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3893,34 +3850,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1340.6799999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>505.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>393.54</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>376.95</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>368.08</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>365.96</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>213.77</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>213.26999999999998</c:v>
+                  <c:v>5211.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1999.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1576.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1529.22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1488.93</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1483.34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>827.59</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>828.47</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>231.64000000000001</c:v>
+                  <c:v>900.14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>188.64</c:v>
+                  <c:v>747.30000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3936,7 +3893,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>256</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3986,34 +3943,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5211.04</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1999.92</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1576.45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1529.22</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1488.93</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1483.34</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>827.59</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>828.47</c:v>
+                  <c:v>1340.6799999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>505.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>393.54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>376.95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>368.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>365.96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>213.77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>213.26999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.14</c:v>
+                  <c:v>231.64000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>747.30000000000007</c:v>
+                  <c:v>188.64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4029,7 +3986,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>512</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4078,29 +4035,35 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="2">
-                  <c:v>6279.2800000000007</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6064.38</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5905.33</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5962.91</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3379.89</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3281.44</c:v>
+                <c:pt idx="0">
+                  <c:v>335.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>127.63999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.38999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95.34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93.33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54.24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>55.22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3582.49</c:v>
+                  <c:v>58.22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3011.57</c:v>
+                  <c:v>48.11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4116,7 +4079,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1024</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4165,26 +4128,35 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="3">
-                  <c:v>24254.35</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>23632.469999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>23889.550000000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13465.76</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>13096.300000000001</c:v>
+                <c:pt idx="0">
+                  <c:v>79.91</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.380000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.61</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.419999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.790000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.780000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14348.41</c:v>
+                  <c:v>14.790000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12003.22</c:v>
+                  <c:v>12.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4200,7 +4172,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1736</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4249,8 +4221,35 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.4700000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.95</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.98</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.67</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.92</c:v>
+                </c:pt>
                 <c:pt idx="9">
-                  <c:v>34714.71</c:v>
+                  <c:v>3.2600000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4267,11 +4266,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="74226176"/>
-        <c:axId val="110773376"/>
+        <c:axId val="57840128"/>
+        <c:axId val="57885248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74226176"/>
+        <c:axId val="57840128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4281,7 +4280,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110773376"/>
+        <c:crossAx val="57885248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4289,7 +4288,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110773376"/>
+        <c:axId val="57885248"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -4327,7 +4326,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74226176"/>
+        <c:crossAx val="57840128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4338,10 +4337,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.79001703751532237"/>
-          <c:y val="8.5494549639162504E-2"/>
+          <c:x val="0.79001693336720002"/>
+          <c:y val="4.6659543526117661E-2"/>
           <c:w val="0.18593812267011031"/>
-          <c:h val="0.71971850959259576"/>
+          <c:h val="0.79091603366614016"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4598,11 +4597,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="110842880"/>
-        <c:axId val="110775680"/>
+        <c:axId val="57841664"/>
+        <c:axId val="57887552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110842880"/>
+        <c:axId val="57841664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4611,7 +4610,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110775680"/>
+        <c:crossAx val="57887552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4619,7 +4618,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110775680"/>
+        <c:axId val="57887552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4630,7 +4629,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110842880"/>
+        <c:crossAx val="57841664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5437,8 +5436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A14:K22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5486,309 +5485,312 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <f>Sheet1!B15*10000</f>
-        <v>20.03</v>
-      </c>
-      <c r="C15">
-        <f>Sheet1!C15*10000</f>
-        <v>8.4700000000000006</v>
-      </c>
-      <c r="D15">
-        <f>Sheet1!D15*10000</f>
-        <v>6.25</v>
-      </c>
-      <c r="E15">
-        <f>Sheet1!E15*10000</f>
-        <v>6.08</v>
-      </c>
-      <c r="F15">
-        <f>Sheet1!F15*10000</f>
-        <v>5.95</v>
-      </c>
-      <c r="G15">
-        <f>Sheet1!G15*10000</f>
-        <v>5.98</v>
-      </c>
-      <c r="H15">
-        <f>Sheet1!H15*10000</f>
-        <v>3.67</v>
-      </c>
-      <c r="I15">
-        <f>Sheet1!I15*10000</f>
-        <v>3.5799999999999996</v>
-      </c>
-      <c r="J15">
-        <f>Sheet1!J15*10000</f>
-        <v>3.92</v>
+        <v>1736</v>
       </c>
       <c r="K15">
-        <f>Sheet1!K15*10000</f>
-        <v>3.2600000000000002</v>
+        <f>Sheet1!K22*10000</f>
+        <v>34714.71</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>32</v>
-      </c>
-      <c r="B16">
-        <f>Sheet1!B16*10000</f>
-        <v>79.91</v>
-      </c>
-      <c r="C16">
-        <f>Sheet1!C16*10000</f>
-        <v>32.380000000000003</v>
-      </c>
-      <c r="D16">
-        <f>Sheet1!D16*10000</f>
-        <v>24.61</v>
+        <v>1024</v>
       </c>
       <c r="E16">
-        <f>Sheet1!E16*10000</f>
-        <v>23.999999999999996</v>
+        <f>Sheet1!E21*10000</f>
+        <v>24254.35</v>
       </c>
       <c r="F16">
-        <f>Sheet1!F16*10000</f>
-        <v>23.45</v>
+        <f>Sheet1!F21*10000</f>
+        <v>23632.469999999998</v>
       </c>
       <c r="G16">
-        <f>Sheet1!G16*10000</f>
-        <v>23.419999999999998</v>
+        <f>Sheet1!G21*10000</f>
+        <v>23889.550000000003</v>
       </c>
       <c r="H16">
-        <f>Sheet1!H16*10000</f>
-        <v>13.790000000000001</v>
+        <f>Sheet1!H21*10000</f>
+        <v>13465.76</v>
       </c>
       <c r="I16">
-        <f>Sheet1!I16*10000</f>
-        <v>13.780000000000001</v>
+        <f>Sheet1!I21*10000</f>
+        <v>13096.300000000001</v>
       </c>
       <c r="J16">
-        <f>Sheet1!J16*10000</f>
-        <v>14.790000000000001</v>
+        <f>Sheet1!J21*10000</f>
+        <v>14348.41</v>
       </c>
       <c r="K16">
-        <f>Sheet1!K16*10000</f>
-        <v>12.25</v>
+        <f>Sheet1!K21*10000</f>
+        <v>12003.22</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>64</v>
-      </c>
-      <c r="B17">
-        <f>Sheet1!B17*10000</f>
-        <v>335.29999999999995</v>
-      </c>
-      <c r="C17">
-        <f>Sheet1!C17*10000</f>
-        <v>127.63999999999999</v>
+        <v>512</v>
       </c>
       <c r="D17">
-        <f>Sheet1!D17*10000</f>
-        <v>100.38999999999999</v>
+        <f>Sheet1!D20*10000</f>
+        <v>6279.2800000000007</v>
       </c>
       <c r="E17">
-        <f>Sheet1!E17*10000</f>
-        <v>97.62</v>
+        <f>Sheet1!E20*10000</f>
+        <v>6064.38</v>
       </c>
       <c r="F17">
-        <f>Sheet1!F17*10000</f>
-        <v>95.34</v>
+        <f>Sheet1!F20*10000</f>
+        <v>5905.33</v>
       </c>
       <c r="G17">
-        <f>Sheet1!G17*10000</f>
-        <v>93.33</v>
+        <f>Sheet1!G20*10000</f>
+        <v>5962.91</v>
       </c>
       <c r="H17">
-        <f>Sheet1!H17*10000</f>
-        <v>54.24</v>
+        <f>Sheet1!H20*10000</f>
+        <v>3379.89</v>
       </c>
       <c r="I17">
-        <f>Sheet1!I17*10000</f>
-        <v>55.22</v>
+        <f>Sheet1!I20*10000</f>
+        <v>3281.44</v>
       </c>
       <c r="J17">
-        <f>Sheet1!J17*10000</f>
-        <v>58.22</v>
+        <f>Sheet1!J20*10000</f>
+        <v>3582.49</v>
       </c>
       <c r="K17">
-        <f>Sheet1!K17*10000</f>
-        <v>48.11</v>
+        <f>Sheet1!K20*10000</f>
+        <v>3011.57</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="B18">
-        <f>Sheet1!B18*10000</f>
-        <v>1340.6799999999998</v>
+        <f>Sheet1!B19*10000</f>
+        <v>5211.04</v>
       </c>
       <c r="C18">
-        <f>Sheet1!C18*10000</f>
-        <v>505.6</v>
+        <f>Sheet1!C19*10000</f>
+        <v>1999.92</v>
       </c>
       <c r="D18">
-        <f>Sheet1!D18*10000</f>
-        <v>393.54</v>
+        <f>Sheet1!D19*10000</f>
+        <v>1576.45</v>
       </c>
       <c r="E18">
-        <f>Sheet1!E18*10000</f>
-        <v>376.95</v>
+        <f>Sheet1!E19*10000</f>
+        <v>1529.22</v>
       </c>
       <c r="F18">
-        <f>Sheet1!F18*10000</f>
-        <v>368.08</v>
+        <f>Sheet1!F19*10000</f>
+        <v>1488.93</v>
       </c>
       <c r="G18">
-        <f>Sheet1!G18*10000</f>
-        <v>365.96</v>
+        <f>Sheet1!G19*10000</f>
+        <v>1483.34</v>
       </c>
       <c r="H18">
-        <f>Sheet1!H18*10000</f>
-        <v>213.77</v>
+        <f>Sheet1!H19*10000</f>
+        <v>827.59</v>
       </c>
       <c r="I18">
-        <f>Sheet1!I18*10000</f>
-        <v>213.26999999999998</v>
+        <f>Sheet1!I19*10000</f>
+        <v>828.47</v>
       </c>
       <c r="J18">
-        <f>Sheet1!J18*10000</f>
-        <v>231.64000000000001</v>
+        <f>Sheet1!J19*10000</f>
+        <v>900.14</v>
       </c>
       <c r="K18">
-        <f>Sheet1!K18*10000</f>
-        <v>188.64</v>
+        <f>Sheet1!K19*10000</f>
+        <v>747.30000000000007</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="B19">
-        <f>Sheet1!B19*10000</f>
-        <v>5211.04</v>
+        <f>Sheet1!B18*10000</f>
+        <v>1340.6799999999998</v>
       </c>
       <c r="C19">
-        <f>Sheet1!C19*10000</f>
-        <v>1999.92</v>
+        <f>Sheet1!C18*10000</f>
+        <v>505.6</v>
       </c>
       <c r="D19">
-        <f>Sheet1!D19*10000</f>
-        <v>1576.45</v>
+        <f>Sheet1!D18*10000</f>
+        <v>393.54</v>
       </c>
       <c r="E19">
-        <f>Sheet1!E19*10000</f>
-        <v>1529.22</v>
+        <f>Sheet1!E18*10000</f>
+        <v>376.95</v>
       </c>
       <c r="F19">
-        <f>Sheet1!F19*10000</f>
-        <v>1488.93</v>
+        <f>Sheet1!F18*10000</f>
+        <v>368.08</v>
       </c>
       <c r="G19">
-        <f>Sheet1!G19*10000</f>
-        <v>1483.34</v>
+        <f>Sheet1!G18*10000</f>
+        <v>365.96</v>
       </c>
       <c r="H19">
-        <f>Sheet1!H19*10000</f>
-        <v>827.59</v>
+        <f>Sheet1!H18*10000</f>
+        <v>213.77</v>
       </c>
       <c r="I19">
-        <f>Sheet1!I19*10000</f>
-        <v>828.47</v>
+        <f>Sheet1!I18*10000</f>
+        <v>213.26999999999998</v>
       </c>
       <c r="J19">
-        <f>Sheet1!J19*10000</f>
-        <v>900.14</v>
+        <f>Sheet1!J18*10000</f>
+        <v>231.64000000000001</v>
       </c>
       <c r="K19">
-        <f>Sheet1!K19*10000</f>
-        <v>747.30000000000007</v>
+        <f>Sheet1!K18*10000</f>
+        <v>188.64</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>512</v>
+        <v>64</v>
+      </c>
+      <c r="B20">
+        <f>Sheet1!B17*10000</f>
+        <v>335.29999999999995</v>
+      </c>
+      <c r="C20">
+        <f>Sheet1!C17*10000</f>
+        <v>127.63999999999999</v>
       </c>
       <c r="D20">
-        <f>Sheet1!D20*10000</f>
-        <v>6279.2800000000007</v>
+        <f>Sheet1!D17*10000</f>
+        <v>100.38999999999999</v>
       </c>
       <c r="E20">
-        <f>Sheet1!E20*10000</f>
-        <v>6064.38</v>
+        <f>Sheet1!E17*10000</f>
+        <v>97.62</v>
       </c>
       <c r="F20">
-        <f>Sheet1!F20*10000</f>
-        <v>5905.33</v>
+        <f>Sheet1!F17*10000</f>
+        <v>95.34</v>
       </c>
       <c r="G20">
-        <f>Sheet1!G20*10000</f>
-        <v>5962.91</v>
+        <f>Sheet1!G17*10000</f>
+        <v>93.33</v>
       </c>
       <c r="H20">
-        <f>Sheet1!H20*10000</f>
-        <v>3379.89</v>
+        <f>Sheet1!H17*10000</f>
+        <v>54.24</v>
       </c>
       <c r="I20">
-        <f>Sheet1!I20*10000</f>
-        <v>3281.44</v>
+        <f>Sheet1!I17*10000</f>
+        <v>55.22</v>
       </c>
       <c r="J20">
-        <f>Sheet1!J20*10000</f>
-        <v>3582.49</v>
+        <f>Sheet1!J17*10000</f>
+        <v>58.22</v>
       </c>
       <c r="K20">
-        <f>Sheet1!K20*10000</f>
-        <v>3011.57</v>
+        <f>Sheet1!K17*10000</f>
+        <v>48.11</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1024</v>
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <f>Sheet1!B16*10000</f>
+        <v>79.91</v>
+      </c>
+      <c r="C21">
+        <f>Sheet1!C16*10000</f>
+        <v>32.380000000000003</v>
+      </c>
+      <c r="D21">
+        <f>Sheet1!D16*10000</f>
+        <v>24.61</v>
       </c>
       <c r="E21">
-        <f>Sheet1!E21*10000</f>
-        <v>24254.35</v>
+        <f>Sheet1!E16*10000</f>
+        <v>23.999999999999996</v>
       </c>
       <c r="F21">
-        <f>Sheet1!F21*10000</f>
-        <v>23632.469999999998</v>
+        <f>Sheet1!F16*10000</f>
+        <v>23.45</v>
       </c>
       <c r="G21">
-        <f>Sheet1!G21*10000</f>
-        <v>23889.550000000003</v>
+        <f>Sheet1!G16*10000</f>
+        <v>23.419999999999998</v>
       </c>
       <c r="H21">
-        <f>Sheet1!H21*10000</f>
-        <v>13465.76</v>
+        <f>Sheet1!H16*10000</f>
+        <v>13.790000000000001</v>
       </c>
       <c r="I21">
-        <f>Sheet1!I21*10000</f>
-        <v>13096.300000000001</v>
+        <f>Sheet1!I16*10000</f>
+        <v>13.780000000000001</v>
       </c>
       <c r="J21">
-        <f>Sheet1!J21*10000</f>
-        <v>14348.41</v>
+        <f>Sheet1!J16*10000</f>
+        <v>14.790000000000001</v>
       </c>
       <c r="K21">
-        <f>Sheet1!K21*10000</f>
-        <v>12003.22</v>
+        <f>Sheet1!K16*10000</f>
+        <v>12.25</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1736</v>
+        <v>16</v>
+      </c>
+      <c r="B22">
+        <f>Sheet1!B15*10000</f>
+        <v>20.03</v>
+      </c>
+      <c r="C22">
+        <f>Sheet1!C15*10000</f>
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="D22">
+        <f>Sheet1!D15*10000</f>
+        <v>6.25</v>
+      </c>
+      <c r="E22">
+        <f>Sheet1!E15*10000</f>
+        <v>6.08</v>
+      </c>
+      <c r="F22">
+        <f>Sheet1!F15*10000</f>
+        <v>5.95</v>
+      </c>
+      <c r="G22">
+        <f>Sheet1!G15*10000</f>
+        <v>5.98</v>
+      </c>
+      <c r="H22">
+        <f>Sheet1!H15*10000</f>
+        <v>3.67</v>
+      </c>
+      <c r="I22">
+        <f>Sheet1!I15*10000</f>
+        <v>3.5799999999999996</v>
+      </c>
+      <c r="J22">
+        <f>Sheet1!J15*10000</f>
+        <v>3.92</v>
       </c>
       <c r="K22">
-        <f>Sheet1!K22*10000</f>
-        <v>34714.71</v>
+        <f>Sheet1!K15*10000</f>
+        <v>3.2600000000000002</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A15:K22">
+    <sortCondition descending="1" ref="A15"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>